<commit_message>
Version 1.0 | Msj:Solucion de multiples if anidados con comprobacion
</commit_message>
<xml_diff>
--- a/Vacantes/Vacantes_ColegioAnguil.xlsx
+++ b/Vacantes/Vacantes_ColegioAnguil.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Rb50b30bb8a854e49"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R358882ddbc874c50"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -113,52 +113,52 @@
     <x:t>Luisa Torres</x:t>
   </x:si>
   <x:si>
+    <x:t>Manuel Vargas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Victoria Rodríguez</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Manuel Ramos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Luisa Fernandez</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Manuel Chavez</x:t>
+  </x:si>
+  <x:si>
     <x:t>Carlos Martinez</x:t>
   </x:si>
   <x:si>
+    <x:t>Hugo González</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Julieta Vargas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ana Sánchez</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Luisa Peralta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Luisa Vargas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Juan Vargas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ana Romero</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Victoria Aguilera</x:t>
+  </x:si>
+  <x:si>
+    <x:t>María Fernandez</x:t>
+  </x:si>
+  <x:si>
     <x:t>Juan González</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Manuel Vargas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Victoria Rodríguez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hugo Martinez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sofia Rodríguez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Julieta Sánchez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Manuel Ramos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>María Fernandez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Luisa Fernandez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Manuel Chavez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>María Gómez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hugo González</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Julieta Vargas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ana Sánchez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Luisa Peralta</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -931,10 +931,10 @@
     </x:row>
     <x:row r="32">
       <x:c r="A32">
-        <x:v>114</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="B32" t="s">
-        <x:v>24</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C32">
         <x:v>8</x:v>
@@ -945,24 +945,24 @@
     </x:row>
     <x:row r="33">
       <x:c r="A33">
-        <x:v>126</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="B33" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C33">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D33">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="34">
       <x:c r="A34">
-        <x:v>127</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="B34" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C34">
         <x:v>8</x:v>
@@ -973,164 +973,164 @@
     </x:row>
     <x:row r="35">
       <x:c r="A35">
-        <x:v>136</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="B35" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C35">
-        <x:v>8</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D35">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="36">
       <x:c r="A36">
-        <x:v>142</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="B36" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C36">
-        <x:v>12</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D36">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="37">
       <x:c r="A37">
-        <x:v>145</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="B37" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C37">
-        <x:v>12</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D37">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="38">
       <x:c r="A38">
-        <x:v>146</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="B38" t="s">
-        <x:v>36</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C38">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D38">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="39">
       <x:c r="A39">
-        <x:v>148</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="B39" t="s">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C39">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D39">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="40">
       <x:c r="A40">
-        <x:v>154</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="B40" t="s">
-        <x:v>39</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C40">
-        <x:v>12</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D40">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="41">
       <x:c r="A41">
-        <x:v>156</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="B41" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C41">
-        <x:v>8</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D41">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="42">
       <x:c r="A42">
-        <x:v>161</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="B42" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C42">
-        <x:v>8</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D42">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="43">
       <x:c r="A43">
-        <x:v>164</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="B43" t="s">
         <x:v>42</x:v>
       </x:c>
       <x:c r="C43">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D43">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="44">
       <x:c r="A44">
-        <x:v>165</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="B44" t="s">
         <x:v>43</x:v>
       </x:c>
       <x:c r="C44">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D44">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="45">
       <x:c r="A45">
-        <x:v>168</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B45" t="s">
-        <x:v>33</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C45">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D45">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="46">
       <x:c r="A46">
-        <x:v>173</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="B46" t="s">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C46">
         <x:v>8</x:v>
@@ -1141,21 +1141,21 @@
     </x:row>
     <x:row r="47">
       <x:c r="A47">
-        <x:v>175</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B47" t="s">
         <x:v>45</x:v>
       </x:c>
       <x:c r="C47">
-        <x:v>7</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D47">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="48">
       <x:c r="A48">
-        <x:v>178</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="B48" t="s">
         <x:v>46</x:v>
@@ -1169,52 +1169,52 @@
     </x:row>
     <x:row r="49">
       <x:c r="A49">
-        <x:v>179</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="B49" t="s">
-        <x:v>31</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C49">
-        <x:v>7</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D49">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="50">
       <x:c r="A50">
-        <x:v>181</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="B50" t="s">
-        <x:v>47</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C50">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D50">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="51">
       <x:c r="A51">
-        <x:v>193</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="B51" t="s">
-        <x:v>48</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C51">
-        <x:v>8</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D51">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="52">
       <x:c r="A52">
-        <x:v>198</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B52" t="s">
-        <x:v>43</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C52">
         <x:v>8</x:v>

</xml_diff>